<commit_message>
fixed ffmpeg automation naming bug
</commit_message>
<xml_diff>
--- a/ffmpeg_automate_filename.xlsx
+++ b/ffmpeg_automate_filename.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\gloriation\Hoopers\cv_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\gloriation\proj\cv_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470F4AE8-CA08-4A71-A229-3BAF04363782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABDE6E0-630F-4253-A88A-8849AED5AF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20190" windowHeight="16335" xr2:uid="{D9E91C62-F7FC-421C-A44A-5F95F8EF8821}"/>
+    <workbookView xWindow="2483" yWindow="2483" windowWidth="18224" windowHeight="11332" xr2:uid="{D9E91C62-F7FC-421C-A44A-5F95F8EF8821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,14 +114,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -499,235 +499,235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A34507F-DE5E-4701-B693-AE0BAD70F591}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="str">
-        <f>_xlfn.CONCAT("ffmpeg -i ", A1,".mp4 -c copy -f h264 ", A1, ".h264 &amp;&amp; ffmpeg -r 30 -i ", A1, ".h264 -c copy ../30fps_input/", A1, "_input.mp4")</f>
-        <v>ffmpeg -i justin_frd1_shoot1.mp4 -c copy -f h264 justin_frd1_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot1.h264 -c copy ../30fps_input/justin_frd1_shoot1_input.mp4</v>
+        <f>_xlfn.CONCAT("ffmpeg -i ", A1,".mp4 -c copy -f h264 ", A1, ".h264 &amp;&amp; ffmpeg -r 30 -i ", A1, ".h264 -c copy ../30fps_input/", A1, "_30fps_input.mp4")</f>
+        <v>ffmpeg -i justin_frd1_shoot1.mp4 -c copy -f h264 justin_frd1_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot1.h264 -c copy ../30fps_input/justin_frd1_shoot1_30fps_input.mp4</v>
       </c>
       <c r="S1" t="str">
         <f>C1</f>
-        <v>ffmpeg -i justin_frd1_shoot1.mp4 -c copy -f h264 justin_frd1_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot1.h264 -c copy ../30fps_input/justin_frd1_shoot1_input.mp4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd1_shoot1.mp4 -c copy -f h264 justin_frd1_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot1.h264 -c copy ../30fps_input/justin_frd1_shoot1_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C17" si="0">_xlfn.CONCAT("ffmpeg -i ", A2,".mp4 -c copy -f h264 ", A2, ".h264 &amp;&amp; ffmpeg -r 30 -i ", A2, ".h264 -c copy ../30fps_input/", A2, "_input.mp4")</f>
-        <v>ffmpeg -i justin_frd1_shoot2.mp4 -c copy -f h264 justin_frd1_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot2.h264 -c copy ../30fps_input/justin_frd1_shoot2_input.mp4</v>
+        <f t="shared" ref="C2:C17" si="0">_xlfn.CONCAT("ffmpeg -i ", A2,".mp4 -c copy -f h264 ", A2, ".h264 &amp;&amp; ffmpeg -r 30 -i ", A2, ".h264 -c copy ../30fps_input/", A2, "_30fps_input.mp4")</f>
+        <v>ffmpeg -i justin_frd1_shoot2.mp4 -c copy -f h264 justin_frd1_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot2.h264 -c copy ../30fps_input/justin_frd1_shoot2_30fps_input.mp4</v>
       </c>
       <c r="S2" t="str">
         <f t="shared" ref="S2:S17" si="1">C2</f>
-        <v>ffmpeg -i justin_frd1_shoot2.mp4 -c copy -f h264 justin_frd1_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot2.h264 -c copy ../30fps_input/justin_frd1_shoot2_input.mp4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd1_shoot2.mp4 -c copy -f h264 justin_frd1_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot2.h264 -c copy ../30fps_input/justin_frd1_shoot2_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd1_shoot3.mp4 -c copy -f h264 justin_frd1_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot3.h264 -c copy ../30fps_input/justin_frd1_shoot3_input.mp4</v>
+        <v>ffmpeg -i justin_frd1_shoot3.mp4 -c copy -f h264 justin_frd1_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot3.h264 -c copy ../30fps_input/justin_frd1_shoot3_30fps_input.mp4</v>
       </c>
       <c r="S3" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd1_shoot3.mp4 -c copy -f h264 justin_frd1_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot3.h264 -c copy ../30fps_input/justin_frd1_shoot3_input.mp4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd1_shoot3.mp4 -c copy -f h264 justin_frd1_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot3.h264 -c copy ../30fps_input/justin_frd1_shoot3_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd1_shoot4.mp4 -c copy -f h264 justin_frd1_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot4.h264 -c copy ../30fps_input/justin_frd1_shoot4_input.mp4</v>
+        <v>ffmpeg -i justin_frd1_shoot4.mp4 -c copy -f h264 justin_frd1_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot4.h264 -c copy ../30fps_input/justin_frd1_shoot4_30fps_input.mp4</v>
       </c>
       <c r="S4" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd1_shoot4.mp4 -c copy -f h264 justin_frd1_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot4.h264 -c copy ../30fps_input/justin_frd1_shoot4_input.mp4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd1_shoot4.mp4 -c copy -f h264 justin_frd1_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot4.h264 -c copy ../30fps_input/justin_frd1_shoot4_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd1_shoot5.mp4 -c copy -f h264 justin_frd1_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot5.h264 -c copy ../30fps_input/justin_frd1_shoot5_input.mp4</v>
+        <v>ffmpeg -i justin_frd1_shoot5.mp4 -c copy -f h264 justin_frd1_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot5.h264 -c copy ../30fps_input/justin_frd1_shoot5_30fps_input.mp4</v>
       </c>
       <c r="S5" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd1_shoot5.mp4 -c copy -f h264 justin_frd1_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot5.h264 -c copy ../30fps_input/justin_frd1_shoot5_input.mp4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd1_shoot5.mp4 -c copy -f h264 justin_frd1_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot5.h264 -c copy ../30fps_input/justin_frd1_shoot5_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot1.mp4 -c copy -f h264 justin_frd2_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot1.h264 -c copy ../30fps_input/justin_frd2_shoot1_input.mp4</v>
+        <v>ffmpeg -i justin_frd2_shoot1.mp4 -c copy -f h264 justin_frd2_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot1.h264 -c copy ../30fps_input/justin_frd2_shoot1_30fps_input.mp4</v>
       </c>
       <c r="S6" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot1.mp4 -c copy -f h264 justin_frd2_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot1.h264 -c copy ../30fps_input/justin_frd2_shoot1_input.mp4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd2_shoot1.mp4 -c copy -f h264 justin_frd2_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot1.h264 -c copy ../30fps_input/justin_frd2_shoot1_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot2.mp4 -c copy -f h264 justin_frd2_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot2.h264 -c copy ../30fps_input/justin_frd2_shoot2_input.mp4</v>
+        <v>ffmpeg -i justin_frd2_shoot2.mp4 -c copy -f h264 justin_frd2_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot2.h264 -c copy ../30fps_input/justin_frd2_shoot2_30fps_input.mp4</v>
       </c>
       <c r="S7" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot2.mp4 -c copy -f h264 justin_frd2_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot2.h264 -c copy ../30fps_input/justin_frd2_shoot2_input.mp4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd2_shoot2.mp4 -c copy -f h264 justin_frd2_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot2.h264 -c copy ../30fps_input/justin_frd2_shoot2_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot3.mp4 -c copy -f h264 justin_frd2_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot3.h264 -c copy ../30fps_input/justin_frd2_shoot3_input.mp4</v>
+        <v>ffmpeg -i justin_frd2_shoot3.mp4 -c copy -f h264 justin_frd2_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot3.h264 -c copy ../30fps_input/justin_frd2_shoot3_30fps_input.mp4</v>
       </c>
       <c r="S8" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot3.mp4 -c copy -f h264 justin_frd2_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot3.h264 -c copy ../30fps_input/justin_frd2_shoot3_input.mp4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd2_shoot3.mp4 -c copy -f h264 justin_frd2_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot3.h264 -c copy ../30fps_input/justin_frd2_shoot3_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot4.mp4 -c copy -f h264 justin_frd2_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot4.h264 -c copy ../30fps_input/justin_frd2_shoot4_input.mp4</v>
+        <v>ffmpeg -i justin_frd2_shoot4.mp4 -c copy -f h264 justin_frd2_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot4.h264 -c copy ../30fps_input/justin_frd2_shoot4_30fps_input.mp4</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot4.mp4 -c copy -f h264 justin_frd2_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot4.h264 -c copy ../30fps_input/justin_frd2_shoot4_input.mp4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd2_shoot4.mp4 -c copy -f h264 justin_frd2_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot4.h264 -c copy ../30fps_input/justin_frd2_shoot4_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot5.mp4 -c copy -f h264 justin_frd2_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot5.h264 -c copy ../30fps_input/justin_frd2_shoot5_input.mp4</v>
+        <v>ffmpeg -i justin_frd2_shoot5.mp4 -c copy -f h264 justin_frd2_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot5.h264 -c copy ../30fps_input/justin_frd2_shoot5_30fps_input.mp4</v>
       </c>
       <c r="S10" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot5.mp4 -c copy -f h264 justin_frd2_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot5.h264 -c copy ../30fps_input/justin_frd2_shoot5_input.mp4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd2_shoot5.mp4 -c copy -f h264 justin_frd2_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot5.h264 -c copy ../30fps_input/justin_frd2_shoot5_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot1.mp4 -c copy -f h264 justin_frd3_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot1.h264 -c copy ../30fps_input/justin_frd3_shoot1_input.mp4</v>
+        <v>ffmpeg -i justin_frd3_shoot1.mp4 -c copy -f h264 justin_frd3_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot1.h264 -c copy ../30fps_input/justin_frd3_shoot1_30fps_input.mp4</v>
       </c>
       <c r="S11" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot1.mp4 -c copy -f h264 justin_frd3_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot1.h264 -c copy ../30fps_input/justin_frd3_shoot1_input.mp4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd3_shoot1.mp4 -c copy -f h264 justin_frd3_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot1.h264 -c copy ../30fps_input/justin_frd3_shoot1_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot2.mp4 -c copy -f h264 justin_frd3_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot2.h264 -c copy ../30fps_input/justin_frd3_shoot2_input.mp4</v>
+        <v>ffmpeg -i justin_frd3_shoot2.mp4 -c copy -f h264 justin_frd3_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot2.h264 -c copy ../30fps_input/justin_frd3_shoot2_30fps_input.mp4</v>
       </c>
       <c r="S12" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot2.mp4 -c copy -f h264 justin_frd3_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot2.h264 -c copy ../30fps_input/justin_frd3_shoot2_input.mp4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd3_shoot2.mp4 -c copy -f h264 justin_frd3_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot2.h264 -c copy ../30fps_input/justin_frd3_shoot2_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot3.mp4 -c copy -f h264 justin_frd3_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot3.h264 -c copy ../30fps_input/justin_frd3_shoot3_input.mp4</v>
+        <v>ffmpeg -i justin_frd3_shoot3.mp4 -c copy -f h264 justin_frd3_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot3.h264 -c copy ../30fps_input/justin_frd3_shoot3_30fps_input.mp4</v>
       </c>
       <c r="S13" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot3.mp4 -c copy -f h264 justin_frd3_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot3.h264 -c copy ../30fps_input/justin_frd3_shoot3_input.mp4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd3_shoot3.mp4 -c copy -f h264 justin_frd3_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot3.h264 -c copy ../30fps_input/justin_frd3_shoot3_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot4.mp4 -c copy -f h264 justin_frd3_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot4.h264 -c copy ../30fps_input/justin_frd3_shoot4_input.mp4</v>
+        <v>ffmpeg -i justin_frd3_shoot4.mp4 -c copy -f h264 justin_frd3_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot4.h264 -c copy ../30fps_input/justin_frd3_shoot4_30fps_input.mp4</v>
       </c>
       <c r="S14" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot4.mp4 -c copy -f h264 justin_frd3_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot4.h264 -c copy ../30fps_input/justin_frd3_shoot4_input.mp4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i justin_frd3_shoot4.mp4 -c copy -f h264 justin_frd3_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot4.h264 -c copy ../30fps_input/justin_frd3_shoot4_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i lee_side_shoot.mp4 -c copy -f h264 lee_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i lee_side_shoot.h264 -c copy ../30fps_input/lee_side_shoot_input.mp4</v>
+        <v>ffmpeg -i lee_side_shoot.mp4 -c copy -f h264 lee_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i lee_side_shoot.h264 -c copy ../30fps_input/lee_side_shoot_30fps_input.mp4</v>
       </c>
       <c r="S15" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i lee_side_shoot.mp4 -c copy -f h264 lee_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i lee_side_shoot.h264 -c copy ../30fps_input/lee_side_shoot_input.mp4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i lee_side_shoot.mp4 -c copy -f h264 lee_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i lee_side_shoot.h264 -c copy ../30fps_input/lee_side_shoot_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i trey_side_shoot.mp4 -c copy -f h264 trey_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i trey_side_shoot.h264 -c copy ../30fps_input/trey_side_shoot_input.mp4</v>
+        <v>ffmpeg -i trey_side_shoot.mp4 -c copy -f h264 trey_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i trey_side_shoot.h264 -c copy ../30fps_input/trey_side_shoot_30fps_input.mp4</v>
       </c>
       <c r="S16" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i trey_side_shoot.mp4 -c copy -f h264 trey_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i trey_side_shoot.h264 -c copy ../30fps_input/trey_side_shoot_input.mp4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
+        <v>ffmpeg -i trey_side_shoot.mp4 -c copy -f h264 trey_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i trey_side_shoot.h264 -c copy ../30fps_input/trey_side_shoot_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i curry_side_shoot.mp4 -c copy -f h264 curry_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i curry_side_shoot.h264 -c copy ../30fps_input/curry_side_shoot_input.mp4</v>
+        <v>ffmpeg -i curry_side_shoot.mp4 -c copy -f h264 curry_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i curry_side_shoot.h264 -c copy ../30fps_input/curry_side_shoot_30fps_input.mp4</v>
       </c>
       <c r="S17" t="str">
         <f t="shared" si="1"/>
-        <v>ffmpeg -i curry_side_shoot.mp4 -c copy -f h264 curry_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i curry_side_shoot.h264 -c copy ../30fps_input/curry_side_shoot_input.mp4</v>
+        <v>ffmpeg -i curry_side_shoot.mp4 -c copy -f h264 curry_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i curry_side_shoot.h264 -c copy ../30fps_input/curry_side_shoot_30fps_input.mp4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added shell script and changed excel
</commit_message>
<xml_diff>
--- a/ffmpeg_automate_filename.xlsx
+++ b/ffmpeg_automate_filename.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\gloriation\proj\cv_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABDE6E0-630F-4253-A88A-8849AED5AF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9049333F-075D-446A-B128-8015522729EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2483" yWindow="2483" windowWidth="18224" windowHeight="11332" xr2:uid="{D9E91C62-F7FC-421C-A44A-5F95F8EF8821}"/>
+    <workbookView xWindow="2250" yWindow="3285" windowWidth="18540" windowHeight="10958" xr2:uid="{D9E91C62-F7FC-421C-A44A-5F95F8EF8821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>justin_frd1_shoot1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,6 +104,9 @@
   <si>
     <t>curry_side_shoot</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/mnt/c/ffmpeg/bin/ffmpeg.exe</t>
   </si>
 </sst>
 </file>
@@ -497,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A34507F-DE5E-4701-B693-AE0BAD70F591}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -509,225 +512,208 @@
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
       <c r="C1" t="str">
-        <f>_xlfn.CONCAT("ffmpeg -i ", A1,".mp4 -c copy -f h264 ", A1, ".h264 &amp;&amp; ffmpeg -r 30 -i ", A1, ".h264 -c copy ../30fps_input/", A1, "_30fps_input.mp4")</f>
-        <v>ffmpeg -i justin_frd1_shoot1.mp4 -c copy -f h264 justin_frd1_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot1.h264 -c copy ../30fps_input/justin_frd1_shoot1_30fps_input.mp4</v>
-      </c>
-      <c r="S1" t="str">
-        <f>C1</f>
-        <v>ffmpeg -i justin_frd1_shoot1.mp4 -c copy -f h264 justin_frd1_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot1.h264 -c copy ../30fps_input/justin_frd1_shoot1_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+        <f>_xlfn.CONCAT(B1, " -i ", A1,".mp4 -c copy -f h264 -y ", A1, ".h264 &amp;&amp; ", B1, " -r 30 -i ", A1, ".h264 -c copy -y ../30fps_input/", A1, "_30fps_input.mp4")</f>
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd1_shoot1.mp4 -c copy -f h264 -y justin_frd1_shoot1.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd1_shoot1.h264 -c copy -y ../30fps_input/justin_frd1_shoot1_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C17" si="0">_xlfn.CONCAT("ffmpeg -i ", A2,".mp4 -c copy -f h264 ", A2, ".h264 &amp;&amp; ffmpeg -r 30 -i ", A2, ".h264 -c copy ../30fps_input/", A2, "_30fps_input.mp4")</f>
-        <v>ffmpeg -i justin_frd1_shoot2.mp4 -c copy -f h264 justin_frd1_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot2.h264 -c copy ../30fps_input/justin_frd1_shoot2_30fps_input.mp4</v>
-      </c>
-      <c r="S2" t="str">
-        <f t="shared" ref="S2:S17" si="1">C2</f>
-        <v>ffmpeg -i justin_frd1_shoot2.mp4 -c copy -f h264 justin_frd1_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot2.h264 -c copy ../30fps_input/justin_frd1_shoot2_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+        <f t="shared" ref="C2:C17" si="0">_xlfn.CONCAT(B2, " -i ", A2,".mp4 -c copy -f h264 -y ", A2, ".h264 &amp;&amp; ", B2, " -r 30 -i ", A2, ".h264 -c copy -y ../30fps_input/", A2, "_30fps_input.mp4")</f>
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd1_shoot2.mp4 -c copy -f h264 -y justin_frd1_shoot2.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd1_shoot2.h264 -c copy -y ../30fps_input/justin_frd1_shoot2_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd1_shoot3.mp4 -c copy -f h264 justin_frd1_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot3.h264 -c copy ../30fps_input/justin_frd1_shoot3_30fps_input.mp4</v>
-      </c>
-      <c r="S3" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd1_shoot3.mp4 -c copy -f h264 justin_frd1_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot3.h264 -c copy ../30fps_input/justin_frd1_shoot3_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd1_shoot3.mp4 -c copy -f h264 -y justin_frd1_shoot3.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd1_shoot3.h264 -c copy -y ../30fps_input/justin_frd1_shoot3_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd1_shoot4.mp4 -c copy -f h264 justin_frd1_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot4.h264 -c copy ../30fps_input/justin_frd1_shoot4_30fps_input.mp4</v>
-      </c>
-      <c r="S4" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd1_shoot4.mp4 -c copy -f h264 justin_frd1_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot4.h264 -c copy ../30fps_input/justin_frd1_shoot4_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd1_shoot4.mp4 -c copy -f h264 -y justin_frd1_shoot4.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd1_shoot4.h264 -c copy -y ../30fps_input/justin_frd1_shoot4_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd1_shoot5.mp4 -c copy -f h264 justin_frd1_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot5.h264 -c copy ../30fps_input/justin_frd1_shoot5_30fps_input.mp4</v>
-      </c>
-      <c r="S5" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd1_shoot5.mp4 -c copy -f h264 justin_frd1_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd1_shoot5.h264 -c copy ../30fps_input/justin_frd1_shoot5_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd1_shoot5.mp4 -c copy -f h264 -y justin_frd1_shoot5.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd1_shoot5.h264 -c copy -y ../30fps_input/justin_frd1_shoot5_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot1.mp4 -c copy -f h264 justin_frd2_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot1.h264 -c copy ../30fps_input/justin_frd2_shoot1_30fps_input.mp4</v>
-      </c>
-      <c r="S6" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot1.mp4 -c copy -f h264 justin_frd2_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot1.h264 -c copy ../30fps_input/justin_frd2_shoot1_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd2_shoot1.mp4 -c copy -f h264 -y justin_frd2_shoot1.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd2_shoot1.h264 -c copy -y ../30fps_input/justin_frd2_shoot1_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot2.mp4 -c copy -f h264 justin_frd2_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot2.h264 -c copy ../30fps_input/justin_frd2_shoot2_30fps_input.mp4</v>
-      </c>
-      <c r="S7" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot2.mp4 -c copy -f h264 justin_frd2_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot2.h264 -c copy ../30fps_input/justin_frd2_shoot2_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd2_shoot2.mp4 -c copy -f h264 -y justin_frd2_shoot2.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd2_shoot2.h264 -c copy -y ../30fps_input/justin_frd2_shoot2_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot3.mp4 -c copy -f h264 justin_frd2_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot3.h264 -c copy ../30fps_input/justin_frd2_shoot3_30fps_input.mp4</v>
-      </c>
-      <c r="S8" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot3.mp4 -c copy -f h264 justin_frd2_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot3.h264 -c copy ../30fps_input/justin_frd2_shoot3_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd2_shoot3.mp4 -c copy -f h264 -y justin_frd2_shoot3.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd2_shoot3.h264 -c copy -y ../30fps_input/justin_frd2_shoot3_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot4.mp4 -c copy -f h264 justin_frd2_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot4.h264 -c copy ../30fps_input/justin_frd2_shoot4_30fps_input.mp4</v>
-      </c>
-      <c r="S9" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot4.mp4 -c copy -f h264 justin_frd2_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot4.h264 -c copy ../30fps_input/justin_frd2_shoot4_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd2_shoot4.mp4 -c copy -f h264 -y justin_frd2_shoot4.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd2_shoot4.h264 -c copy -y ../30fps_input/justin_frd2_shoot4_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd2_shoot5.mp4 -c copy -f h264 justin_frd2_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot5.h264 -c copy ../30fps_input/justin_frd2_shoot5_30fps_input.mp4</v>
-      </c>
-      <c r="S10" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd2_shoot5.mp4 -c copy -f h264 justin_frd2_shoot5.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd2_shoot5.h264 -c copy ../30fps_input/justin_frd2_shoot5_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd2_shoot5.mp4 -c copy -f h264 -y justin_frd2_shoot5.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd2_shoot5.h264 -c copy -y ../30fps_input/justin_frd2_shoot5_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot1.mp4 -c copy -f h264 justin_frd3_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot1.h264 -c copy ../30fps_input/justin_frd3_shoot1_30fps_input.mp4</v>
-      </c>
-      <c r="S11" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot1.mp4 -c copy -f h264 justin_frd3_shoot1.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot1.h264 -c copy ../30fps_input/justin_frd3_shoot1_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd3_shoot1.mp4 -c copy -f h264 -y justin_frd3_shoot1.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd3_shoot1.h264 -c copy -y ../30fps_input/justin_frd3_shoot1_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot2.mp4 -c copy -f h264 justin_frd3_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot2.h264 -c copy ../30fps_input/justin_frd3_shoot2_30fps_input.mp4</v>
-      </c>
-      <c r="S12" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot2.mp4 -c copy -f h264 justin_frd3_shoot2.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot2.h264 -c copy ../30fps_input/justin_frd3_shoot2_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd3_shoot2.mp4 -c copy -f h264 -y justin_frd3_shoot2.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd3_shoot2.h264 -c copy -y ../30fps_input/justin_frd3_shoot2_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot3.mp4 -c copy -f h264 justin_frd3_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot3.h264 -c copy ../30fps_input/justin_frd3_shoot3_30fps_input.mp4</v>
-      </c>
-      <c r="S13" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot3.mp4 -c copy -f h264 justin_frd3_shoot3.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot3.h264 -c copy ../30fps_input/justin_frd3_shoot3_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd3_shoot3.mp4 -c copy -f h264 -y justin_frd3_shoot3.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd3_shoot3.h264 -c copy -y ../30fps_input/justin_frd3_shoot3_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i justin_frd3_shoot4.mp4 -c copy -f h264 justin_frd3_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot4.h264 -c copy ../30fps_input/justin_frd3_shoot4_30fps_input.mp4</v>
-      </c>
-      <c r="S14" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i justin_frd3_shoot4.mp4 -c copy -f h264 justin_frd3_shoot4.h264 &amp;&amp; ffmpeg -r 30 -i justin_frd3_shoot4.h264 -c copy ../30fps_input/justin_frd3_shoot4_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i justin_frd3_shoot4.mp4 -c copy -f h264 -y justin_frd3_shoot4.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i justin_frd3_shoot4.h264 -c copy -y ../30fps_input/justin_frd3_shoot4_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i lee_side_shoot.mp4 -c copy -f h264 lee_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i lee_side_shoot.h264 -c copy ../30fps_input/lee_side_shoot_30fps_input.mp4</v>
-      </c>
-      <c r="S15" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i lee_side_shoot.mp4 -c copy -f h264 lee_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i lee_side_shoot.h264 -c copy ../30fps_input/lee_side_shoot_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i lee_side_shoot.mp4 -c copy -f h264 -y lee_side_shoot.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i lee_side_shoot.h264 -c copy -y ../30fps_input/lee_side_shoot_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i trey_side_shoot.mp4 -c copy -f h264 trey_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i trey_side_shoot.h264 -c copy ../30fps_input/trey_side_shoot_30fps_input.mp4</v>
-      </c>
-      <c r="S16" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i trey_side_shoot.mp4 -c copy -f h264 trey_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i trey_side_shoot.h264 -c copy ../30fps_input/trey_side_shoot_30fps_input.mp4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i trey_side_shoot.mp4 -c copy -f h264 -y trey_side_shoot.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i trey_side_shoot.h264 -c copy -y ../30fps_input/trey_side_shoot_30fps_input.mp4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>ffmpeg -i curry_side_shoot.mp4 -c copy -f h264 curry_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i curry_side_shoot.h264 -c copy ../30fps_input/curry_side_shoot_30fps_input.mp4</v>
-      </c>
-      <c r="S17" t="str">
-        <f t="shared" si="1"/>
-        <v>ffmpeg -i curry_side_shoot.mp4 -c copy -f h264 curry_side_shoot.h264 &amp;&amp; ffmpeg -r 30 -i curry_side_shoot.h264 -c copy ../30fps_input/curry_side_shoot_30fps_input.mp4</v>
+        <v>/mnt/c/ffmpeg/bin/ffmpeg.exe -i curry_side_shoot.mp4 -c copy -f h264 -y curry_side_shoot.h264 &amp;&amp; /mnt/c/ffmpeg/bin/ffmpeg.exe -r 30 -i curry_side_shoot.h264 -c copy -y ../30fps_input/curry_side_shoot_30fps_input.mp4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>